<commit_message>
Added arabic lang to master-data xlxs sheets
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/app_detail.xlsx
+++ b/mosip_master/xlsx/app_detail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -116,6 +116,45 @@
   </si>
   <si>
     <t xml:space="preserve">Portail Web pour les services de génération de post-ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">التسجيل المسبق</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بوابة الويب للتسجيلات المسبقة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عميل التسجيل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تطبيق سطح المكتب للتسجيلات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">معالج التسجيل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">طلب عملية ما بعد التسجيل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مصادقة الهوية</t>
+  </si>
+  <si>
+    <t xml:space="preserve">طلب مصادقة مزود خدمة الطرف الثالث</t>
+  </si>
+  <si>
+    <t xml:space="preserve">معرف التحكم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بوابة الويب لتكوين التطبيقات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بوابة المقيمين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بوابة الويب لخدمات إنشاء معرف البريد</t>
   </si>
 </sst>
 </file>
@@ -206,7 +245,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,6 +266,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,15 +287,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.04"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.43"/>
   </cols>
   <sheetData>
@@ -477,6 +522,109 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>10001</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>10003</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>10005</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>10007</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>10009</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>10011</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Revert "Added arabic lang to master-data xlxs sheets"
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/app_detail.xlsx
+++ b/mosip_master/xlsx/app_detail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -116,45 +116,6 @@
   </si>
   <si>
     <t xml:space="preserve">Portail Web pour les services de génération de post-ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">التسجيل المسبق</t>
-  </si>
-  <si>
-    <t xml:space="preserve">بوابة الويب للتسجيلات المسبقة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عميل التسجيل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">تطبيق سطح المكتب للتسجيلات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">معالج التسجيل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">طلب عملية ما بعد التسجيل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">مصادقة الهوية</t>
-  </si>
-  <si>
-    <t xml:space="preserve">طلب مصادقة مزود خدمة الطرف الثالث</t>
-  </si>
-  <si>
-    <t xml:space="preserve">معرف التحكم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">بوابة الويب لتكوين التطبيقات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">بوابة المقيمين</t>
-  </si>
-  <si>
-    <t xml:space="preserve">بوابة الويب لخدمات إنشاء معرف البريد</t>
   </si>
 </sst>
 </file>
@@ -245,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,10 +225,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -287,17 +244,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14:D19"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.43"/>
   </cols>
   <sheetData>
@@ -522,109 +477,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>10001</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>10003</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>10005</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>10007</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>10009</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="n">
-        <v>10011</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>